<commit_message>
4/4/22 update lan 2
</commit_message>
<xml_diff>
--- a/220329 HTK UV LED Controller Project sheet.xlsx
+++ b/220329 HTK UV LED Controller Project sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f734f300cb83d8b/HTK DAIAN/MORITEX/UV LED CONTROLLER/HTK LED UV Project Plan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="278" documentId="8_{5226F4C7-42C1-4648-860A-165D07E2F74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67488277-E78F-4E1B-BDDD-71A41B2A14DD}"/>
+  <xr:revisionPtr revIDLastSave="288" documentId="8_{5226F4C7-42C1-4648-860A-165D07E2F74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E2BF5C8-46EA-4EBB-B49F-4E141ABB1D50}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="323">
   <si>
     <t>Select a period to highlight at right.  A legend describing the charting follows.</t>
   </si>
@@ -1122,7 +1122,7 @@
     <numFmt numFmtId="164" formatCode="0.00_ "/>
     <numFmt numFmtId="165" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="43">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -1428,6 +1428,11 @@
     <font>
       <sz val="20"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1855,7 +1860,7 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="191">
+  <cellXfs count="192">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2244,6 +2249,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="41" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="42" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2420,10 +2432,6 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="41" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="21">
@@ -3657,10 +3665,10 @@
   <dimension ref="A1:GV112"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="18" ySplit="8" topLeftCell="S33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="18" ySplit="8" topLeftCell="S9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="O1" sqref="O1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="G45" sqref="G45"/>
+      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1"/>
@@ -3715,45 +3723,45 @@
       <c r="S1" s="4"/>
       <c r="T1" s="4"/>
       <c r="U1" s="5"/>
-      <c r="V1" s="176" t="s">
+      <c r="V1" s="179" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="177"/>
-      <c r="X1" s="177"/>
-      <c r="Y1" s="177"/>
-      <c r="Z1" s="177"/>
-      <c r="AA1" s="177"/>
+      <c r="W1" s="180"/>
+      <c r="X1" s="180"/>
+      <c r="Y1" s="180"/>
+      <c r="Z1" s="180"/>
+      <c r="AA1" s="180"/>
       <c r="AB1" s="52">
         <v>1</v>
       </c>
       <c r="AD1" s="51"/>
-      <c r="AE1" s="172" t="s">
+      <c r="AE1" s="175" t="s">
         <v>3</v>
       </c>
-      <c r="AF1" s="173"/>
-      <c r="AG1" s="173"/>
-      <c r="AH1" s="173"/>
-      <c r="AI1" s="174"/>
+      <c r="AF1" s="176"/>
+      <c r="AG1" s="176"/>
+      <c r="AH1" s="176"/>
+      <c r="AI1" s="177"/>
       <c r="AJ1" s="54"/>
-      <c r="AK1" s="172" t="s">
+      <c r="AK1" s="175" t="s">
         <v>4</v>
       </c>
-      <c r="AL1" s="175"/>
-      <c r="AM1" s="175"/>
-      <c r="AN1" s="174"/>
+      <c r="AL1" s="178"/>
+      <c r="AM1" s="178"/>
+      <c r="AN1" s="177"/>
       <c r="AO1" s="55"/>
-      <c r="AP1" s="176" t="s">
+      <c r="AP1" s="179" t="s">
         <v>5</v>
       </c>
-      <c r="AQ1" s="177"/>
-      <c r="AR1" s="177"/>
-      <c r="AS1" s="178"/>
+      <c r="AQ1" s="180"/>
+      <c r="AR1" s="180"/>
+      <c r="AS1" s="181"/>
       <c r="AT1" s="56"/>
-      <c r="AU1" s="176" t="s">
+      <c r="AU1" s="179" t="s">
         <v>2</v>
       </c>
-      <c r="AV1" s="177"/>
-      <c r="AW1" s="177"/>
+      <c r="AV1" s="180"/>
+      <c r="AW1" s="180"/>
     </row>
     <row r="2" spans="1:204" ht="53.25" customHeight="1">
       <c r="A2" s="36" t="s">
@@ -4201,47 +4209,47 @@
       <c r="GV5" s="76"/>
     </row>
     <row r="6" spans="1:204" s="6" customFormat="1" ht="44.25" customHeight="1">
-      <c r="B6" s="166" t="s">
+      <c r="B6" s="169" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="167"/>
-      <c r="D6" s="167"/>
-      <c r="E6" s="168"/>
-      <c r="F6" s="181" t="s">
+      <c r="C6" s="170"/>
+      <c r="D6" s="170"/>
+      <c r="E6" s="171"/>
+      <c r="F6" s="184" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="185" t="s">
+      <c r="G6" s="188" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="179" t="s">
+      <c r="H6" s="182" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="179" t="s">
+      <c r="I6" s="182" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="187" t="s">
+      <c r="J6" s="190" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="179" t="s">
+      <c r="K6" s="182" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="179" t="s">
+      <c r="L6" s="182" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="179" t="s">
+      <c r="M6" s="182" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="179" t="s">
+      <c r="N6" s="182" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="179" t="s">
+      <c r="O6" s="182" t="s">
         <v>23</v>
       </c>
-      <c r="P6" s="183" t="s">
+      <c r="P6" s="186" t="s">
         <v>24</v>
       </c>
-      <c r="Q6" s="183"/>
-      <c r="R6" s="183" t="s">
+      <c r="Q6" s="186"/>
+      <c r="R6" s="186" t="s">
         <v>25</v>
       </c>
       <c r="S6" s="93"/>
@@ -4438,23 +4446,23 @@
       <c r="GV6" s="103"/>
     </row>
     <row r="7" spans="1:204" ht="15.75" customHeight="1">
-      <c r="B7" s="169"/>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="171"/>
-      <c r="F7" s="182"/>
-      <c r="G7" s="186"/>
-      <c r="H7" s="180"/>
-      <c r="I7" s="180"/>
-      <c r="J7" s="188"/>
-      <c r="K7" s="180"/>
-      <c r="L7" s="180"/>
-      <c r="M7" s="180"/>
-      <c r="N7" s="180"/>
-      <c r="O7" s="180"/>
-      <c r="P7" s="184"/>
-      <c r="Q7" s="184"/>
-      <c r="R7" s="184"/>
+      <c r="B7" s="172"/>
+      <c r="C7" s="173"/>
+      <c r="D7" s="173"/>
+      <c r="E7" s="174"/>
+      <c r="F7" s="185"/>
+      <c r="G7" s="189"/>
+      <c r="H7" s="183"/>
+      <c r="I7" s="183"/>
+      <c r="J7" s="191"/>
+      <c r="K7" s="183"/>
+      <c r="L7" s="183"/>
+      <c r="M7" s="183"/>
+      <c r="N7" s="183"/>
+      <c r="O7" s="183"/>
+      <c r="P7" s="187"/>
+      <c r="Q7" s="187"/>
+      <c r="R7" s="187"/>
       <c r="S7" s="28">
         <v>1</v>
       </c>
@@ -5533,12 +5541,12 @@
       <c r="A9" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="145" t="s">
+      <c r="B9" s="148" t="s">
         <v>321</v>
       </c>
-      <c r="C9" s="146"/>
-      <c r="D9" s="146"/>
-      <c r="E9" s="146"/>
+      <c r="C9" s="149"/>
+      <c r="D9" s="149"/>
+      <c r="E9" s="149"/>
       <c r="F9" s="59"/>
       <c r="G9" s="60" t="s">
         <v>30</v>
@@ -5746,12 +5754,12 @@
       <c r="GV9" s="13"/>
     </row>
     <row r="10" spans="1:204" ht="30" customHeight="1">
-      <c r="B10" s="144" t="s">
+      <c r="B10" s="147" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="133"/>
-      <c r="D10" s="133"/>
-      <c r="E10" s="134"/>
+      <c r="C10" s="136"/>
+      <c r="D10" s="136"/>
+      <c r="E10" s="137"/>
       <c r="F10" s="23" t="s">
         <v>31</v>
       </c>
@@ -5967,12 +5975,12 @@
       <c r="GV10" s="13"/>
     </row>
     <row r="11" spans="1:204" ht="30" customHeight="1">
-      <c r="B11" s="130" t="s">
+      <c r="B11" s="133" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="131"/>
-      <c r="D11" s="131"/>
-      <c r="E11" s="132"/>
+      <c r="C11" s="134"/>
+      <c r="D11" s="134"/>
+      <c r="E11" s="135"/>
       <c r="F11" s="23"/>
       <c r="G11" s="26" t="s">
         <v>73</v>
@@ -6178,20 +6186,20 @@
       <c r="GV11" s="13"/>
     </row>
     <row r="12" spans="1:204" ht="36.75" customHeight="1">
-      <c r="B12" s="139"/>
-      <c r="C12" s="130" t="s">
+      <c r="B12" s="142"/>
+      <c r="C12" s="133" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="131"/>
-      <c r="E12" s="132"/>
+      <c r="D12" s="134"/>
+      <c r="E12" s="135"/>
       <c r="F12" s="23"/>
-      <c r="G12" s="189" t="s">
+      <c r="G12" s="130" t="s">
         <v>322</v>
       </c>
       <c r="H12" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="I12" s="190">
+      <c r="I12" s="131">
         <v>44657</v>
       </c>
       <c r="J12" s="14">
@@ -6395,12 +6403,12 @@
       <c r="GV12" s="13"/>
     </row>
     <row r="13" spans="1:204" ht="37.5" hidden="1" customHeight="1">
-      <c r="B13" s="140"/>
-      <c r="C13" s="130" t="s">
+      <c r="B13" s="143"/>
+      <c r="C13" s="133" t="s">
         <v>79</v>
       </c>
-      <c r="D13" s="131"/>
-      <c r="E13" s="132"/>
+      <c r="D13" s="134"/>
+      <c r="E13" s="135"/>
       <c r="F13" s="23"/>
       <c r="G13" s="26"/>
       <c r="H13" s="14" t="s">
@@ -6612,12 +6620,12 @@
       <c r="GV13" s="105"/>
     </row>
     <row r="14" spans="1:204" ht="26.25" hidden="1">
-      <c r="B14" s="140"/>
-      <c r="C14" s="130" t="s">
+      <c r="B14" s="143"/>
+      <c r="C14" s="133" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="131"/>
-      <c r="E14" s="132"/>
+      <c r="D14" s="134"/>
+      <c r="E14" s="135"/>
       <c r="F14" s="23"/>
       <c r="G14" s="26"/>
       <c r="H14" s="14" t="s">
@@ -6827,19 +6835,19 @@
       <c r="GV14" s="13"/>
     </row>
     <row r="15" spans="1:204" ht="26.25">
-      <c r="B15" s="140"/>
-      <c r="C15" s="130" t="s">
+      <c r="B15" s="143"/>
+      <c r="C15" s="133" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="131"/>
-      <c r="E15" s="132"/>
+      <c r="D15" s="134"/>
+      <c r="E15" s="135"/>
       <c r="F15" s="23"/>
       <c r="G15" s="26"/>
       <c r="H15" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="I15" s="190">
-        <v>44656</v>
+      <c r="I15" s="131">
+        <v>44657</v>
       </c>
       <c r="J15" s="14">
         <v>6</v>
@@ -7042,19 +7050,19 @@
       <c r="GV15" s="13"/>
     </row>
     <row r="16" spans="1:204" ht="26.25">
-      <c r="B16" s="140"/>
-      <c r="C16" s="130" t="s">
+      <c r="B16" s="143"/>
+      <c r="C16" s="133" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="131"/>
-      <c r="E16" s="132"/>
+      <c r="D16" s="134"/>
+      <c r="E16" s="135"/>
       <c r="F16" s="23"/>
       <c r="G16" s="26"/>
       <c r="H16" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="I16" s="41">
-        <v>44656</v>
+      <c r="I16" s="131">
+        <v>44657</v>
       </c>
       <c r="J16" s="14">
         <v>6</v>
@@ -7257,19 +7265,19 @@
       <c r="GV16" s="13"/>
     </row>
     <row r="17" spans="2:204" ht="34.5" customHeight="1">
-      <c r="B17" s="141"/>
-      <c r="C17" s="130" t="s">
+      <c r="B17" s="144"/>
+      <c r="C17" s="133" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="131"/>
-      <c r="E17" s="132"/>
+      <c r="D17" s="134"/>
+      <c r="E17" s="135"/>
       <c r="F17" s="23"/>
       <c r="G17" s="26"/>
       <c r="H17" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="I17" s="41">
-        <v>44656</v>
+      <c r="I17" s="131">
+        <v>44657</v>
       </c>
       <c r="J17" s="14">
         <v>7</v>
@@ -7472,12 +7480,12 @@
       <c r="GV17" s="13"/>
     </row>
     <row r="18" spans="2:204" ht="26.25">
-      <c r="B18" s="130" t="s">
+      <c r="B18" s="133" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="131"/>
-      <c r="D18" s="131"/>
-      <c r="E18" s="132"/>
+      <c r="C18" s="134"/>
+      <c r="D18" s="134"/>
+      <c r="E18" s="135"/>
       <c r="F18" s="23"/>
       <c r="G18" s="26" t="s">
         <v>74</v>
@@ -7683,20 +7691,20 @@
       <c r="GV18" s="13"/>
     </row>
     <row r="19" spans="2:204" ht="39" customHeight="1">
-      <c r="B19" s="139"/>
-      <c r="C19" s="130" t="s">
+      <c r="B19" s="142"/>
+      <c r="C19" s="133" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="131"/>
-      <c r="E19" s="132"/>
+      <c r="D19" s="134"/>
+      <c r="E19" s="135"/>
       <c r="F19" s="23"/>
-      <c r="G19" s="189" t="s">
+      <c r="G19" s="130" t="s">
         <v>322</v>
       </c>
       <c r="H19" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="I19" s="190">
+      <c r="I19" s="131">
         <v>44657</v>
       </c>
       <c r="J19" s="14">
@@ -7900,12 +7908,12 @@
       <c r="GV19" s="13"/>
     </row>
     <row r="20" spans="2:204" ht="34.5" customHeight="1">
-      <c r="B20" s="140"/>
-      <c r="C20" s="130" t="s">
+      <c r="B20" s="143"/>
+      <c r="C20" s="133" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="131"/>
-      <c r="E20" s="132"/>
+      <c r="D20" s="134"/>
+      <c r="E20" s="135"/>
       <c r="F20" s="23"/>
       <c r="G20" s="26"/>
       <c r="H20" s="14" t="s">
@@ -8115,12 +8123,12 @@
       <c r="GV20" s="13"/>
     </row>
     <row r="21" spans="2:204" ht="34.5" customHeight="1">
-      <c r="B21" s="140"/>
-      <c r="C21" s="130" t="s">
+      <c r="B21" s="143"/>
+      <c r="C21" s="133" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="131"/>
-      <c r="E21" s="132"/>
+      <c r="D21" s="134"/>
+      <c r="E21" s="135"/>
       <c r="F21" s="23"/>
       <c r="G21" s="26"/>
       <c r="H21" s="14" t="s">
@@ -8328,12 +8336,12 @@
       <c r="GV21" s="13"/>
     </row>
     <row r="22" spans="2:204" ht="37.5" customHeight="1">
-      <c r="B22" s="141"/>
-      <c r="C22" s="130" t="s">
+      <c r="B22" s="144"/>
+      <c r="C22" s="133" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="131"/>
-      <c r="E22" s="132"/>
+      <c r="D22" s="134"/>
+      <c r="E22" s="135"/>
       <c r="F22" s="23"/>
       <c r="G22" s="26"/>
       <c r="H22" s="14" t="s">
@@ -8541,12 +8549,12 @@
       <c r="GV22" s="13"/>
     </row>
     <row r="23" spans="2:204" ht="26.25">
-      <c r="B23" s="130" t="s">
+      <c r="B23" s="133" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="131"/>
-      <c r="D23" s="131"/>
-      <c r="E23" s="132"/>
+      <c r="C23" s="134"/>
+      <c r="D23" s="134"/>
+      <c r="E23" s="135"/>
       <c r="F23" s="23"/>
       <c r="G23" s="26" t="s">
         <v>75</v>
@@ -8752,20 +8760,20 @@
       <c r="GV23" s="13"/>
     </row>
     <row r="24" spans="2:204" ht="26.25">
-      <c r="B24" s="139"/>
-      <c r="C24" s="130" t="s">
+      <c r="B24" s="142"/>
+      <c r="C24" s="133" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="131"/>
-      <c r="E24" s="132"/>
+      <c r="D24" s="134"/>
+      <c r="E24" s="135"/>
       <c r="F24" s="23"/>
-      <c r="G24" s="189" t="s">
+      <c r="G24" s="130" t="s">
         <v>322</v>
       </c>
       <c r="H24" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="I24" s="190">
+      <c r="I24" s="131">
         <v>44657</v>
       </c>
       <c r="J24" s="14">
@@ -8969,12 +8977,12 @@
       <c r="GV24" s="13"/>
     </row>
     <row r="25" spans="2:204" ht="36.75" customHeight="1">
-      <c r="B25" s="140"/>
-      <c r="C25" s="130" t="s">
+      <c r="B25" s="143"/>
+      <c r="C25" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="D25" s="131"/>
-      <c r="E25" s="132"/>
+      <c r="D25" s="134"/>
+      <c r="E25" s="135"/>
       <c r="F25" s="23"/>
       <c r="G25" s="26"/>
       <c r="H25" s="14" t="s">
@@ -9182,12 +9190,12 @@
       <c r="GV25" s="13"/>
     </row>
     <row r="26" spans="2:204" ht="26.25">
-      <c r="B26" s="140"/>
-      <c r="C26" s="130" t="s">
+      <c r="B26" s="143"/>
+      <c r="C26" s="133" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="131"/>
-      <c r="E26" s="132"/>
+      <c r="D26" s="134"/>
+      <c r="E26" s="135"/>
       <c r="F26" s="23"/>
       <c r="G26" s="26"/>
       <c r="H26" s="14" t="s">
@@ -9395,12 +9403,12 @@
       <c r="GV26" s="13"/>
     </row>
     <row r="27" spans="2:204" ht="26.25">
-      <c r="B27" s="140"/>
-      <c r="C27" s="130" t="s">
+      <c r="B27" s="143"/>
+      <c r="C27" s="133" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="131"/>
-      <c r="E27" s="132"/>
+      <c r="D27" s="134"/>
+      <c r="E27" s="135"/>
       <c r="F27" s="23"/>
       <c r="G27" s="26"/>
       <c r="H27" s="14" t="s">
@@ -9608,12 +9616,12 @@
       <c r="GV27" s="13"/>
     </row>
     <row r="28" spans="2:204" ht="26.25">
-      <c r="B28" s="141"/>
-      <c r="C28" s="130" t="s">
+      <c r="B28" s="144"/>
+      <c r="C28" s="133" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="131"/>
-      <c r="E28" s="132"/>
+      <c r="D28" s="134"/>
+      <c r="E28" s="135"/>
       <c r="F28" s="23"/>
       <c r="G28" s="26"/>
       <c r="H28" s="14" t="s">
@@ -9821,12 +9829,12 @@
       <c r="GV28" s="13"/>
     </row>
     <row r="29" spans="2:204" ht="26.25">
-      <c r="B29" s="130" t="s">
+      <c r="B29" s="133" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="131"/>
-      <c r="D29" s="131"/>
-      <c r="E29" s="132"/>
+      <c r="C29" s="134"/>
+      <c r="D29" s="134"/>
+      <c r="E29" s="135"/>
       <c r="F29" s="23"/>
       <c r="G29" s="26" t="s">
         <v>76</v>
@@ -10032,20 +10040,20 @@
       <c r="GV29" s="13"/>
     </row>
     <row r="30" spans="2:204" ht="33.75" customHeight="1">
-      <c r="B30" s="139"/>
-      <c r="C30" s="130" t="s">
+      <c r="B30" s="142"/>
+      <c r="C30" s="133" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="131"/>
-      <c r="E30" s="132"/>
+      <c r="D30" s="134"/>
+      <c r="E30" s="135"/>
       <c r="F30" s="23"/>
-      <c r="G30" s="189" t="s">
+      <c r="G30" s="130" t="s">
         <v>322</v>
       </c>
       <c r="H30" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="I30" s="190">
+      <c r="I30" s="131">
         <v>44657</v>
       </c>
       <c r="J30" s="14">
@@ -10249,12 +10257,12 @@
       <c r="GV30" s="13"/>
     </row>
     <row r="31" spans="2:204" ht="36.75" customHeight="1">
-      <c r="B31" s="140"/>
-      <c r="C31" s="130" t="s">
+      <c r="B31" s="143"/>
+      <c r="C31" s="133" t="s">
         <v>82</v>
       </c>
-      <c r="D31" s="131"/>
-      <c r="E31" s="132"/>
+      <c r="D31" s="134"/>
+      <c r="E31" s="135"/>
       <c r="F31" s="23"/>
       <c r="G31" s="26"/>
       <c r="H31" s="14" t="s">
@@ -10462,12 +10470,12 @@
       <c r="GV31" s="13"/>
     </row>
     <row r="32" spans="2:204" ht="26.25">
-      <c r="B32" s="140"/>
-      <c r="C32" s="130" t="s">
+      <c r="B32" s="143"/>
+      <c r="C32" s="133" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="131"/>
-      <c r="E32" s="132"/>
+      <c r="D32" s="134"/>
+      <c r="E32" s="135"/>
       <c r="F32" s="23"/>
       <c r="G32" s="26"/>
       <c r="H32" s="14" t="s">
@@ -10675,12 +10683,12 @@
       <c r="GV32" s="13"/>
     </row>
     <row r="33" spans="2:204" ht="26.25">
-      <c r="B33" s="140"/>
-      <c r="C33" s="130" t="s">
+      <c r="B33" s="143"/>
+      <c r="C33" s="133" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="131"/>
-      <c r="E33" s="132"/>
+      <c r="D33" s="134"/>
+      <c r="E33" s="135"/>
       <c r="F33" s="23"/>
       <c r="G33" s="26"/>
       <c r="H33" s="14" t="s">
@@ -10888,12 +10896,12 @@
       <c r="GV33" s="13"/>
     </row>
     <row r="34" spans="2:204" ht="26.25">
-      <c r="B34" s="140"/>
-      <c r="C34" s="130" t="s">
+      <c r="B34" s="143"/>
+      <c r="C34" s="133" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="131"/>
-      <c r="E34" s="132"/>
+      <c r="D34" s="134"/>
+      <c r="E34" s="135"/>
       <c r="F34" s="23"/>
       <c r="G34" s="26" t="s">
         <v>151</v>
@@ -11103,12 +11111,12 @@
       <c r="GV34" s="13"/>
     </row>
     <row r="35" spans="2:204" ht="35.25" customHeight="1">
-      <c r="B35" s="141"/>
-      <c r="C35" s="130" t="s">
+      <c r="B35" s="144"/>
+      <c r="C35" s="133" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="131"/>
-      <c r="E35" s="132"/>
+      <c r="D35" s="134"/>
+      <c r="E35" s="135"/>
       <c r="F35" s="23"/>
       <c r="G35" s="26"/>
       <c r="H35" s="14" t="s">
@@ -11316,12 +11324,12 @@
       <c r="GV35" s="13"/>
     </row>
     <row r="36" spans="2:204" ht="35.25" customHeight="1">
-      <c r="B36" s="130" t="s">
+      <c r="B36" s="133" t="s">
         <v>293</v>
       </c>
-      <c r="C36" s="131"/>
-      <c r="D36" s="131"/>
-      <c r="E36" s="132"/>
+      <c r="C36" s="134"/>
+      <c r="D36" s="134"/>
+      <c r="E36" s="135"/>
       <c r="F36" s="23"/>
       <c r="G36" s="26" t="s">
         <v>294</v>
@@ -11531,12 +11539,12 @@
       <c r="GV36" s="13"/>
     </row>
     <row r="37" spans="2:204" ht="35.25" customHeight="1">
-      <c r="B37" s="135"/>
-      <c r="C37" s="131" t="s">
+      <c r="B37" s="138"/>
+      <c r="C37" s="134" t="s">
         <v>295</v>
       </c>
-      <c r="D37" s="131"/>
-      <c r="E37" s="132"/>
+      <c r="D37" s="134"/>
+      <c r="E37" s="135"/>
       <c r="F37" s="23"/>
       <c r="G37" s="26"/>
       <c r="H37" s="14" t="s">
@@ -11744,12 +11752,12 @@
       <c r="GV37" s="13"/>
     </row>
     <row r="38" spans="2:204" ht="35.25" customHeight="1">
-      <c r="B38" s="136"/>
-      <c r="C38" s="131" t="s">
+      <c r="B38" s="139"/>
+      <c r="C38" s="134" t="s">
         <v>296</v>
       </c>
-      <c r="D38" s="131"/>
-      <c r="E38" s="132"/>
+      <c r="D38" s="134"/>
+      <c r="E38" s="135"/>
       <c r="F38" s="23"/>
       <c r="G38" s="26"/>
       <c r="H38" s="14" t="s">
@@ -11957,12 +11965,12 @@
       <c r="GV38" s="13"/>
     </row>
     <row r="39" spans="2:204" ht="26.25">
-      <c r="B39" s="144" t="s">
+      <c r="B39" s="147" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="133"/>
-      <c r="D39" s="133"/>
-      <c r="E39" s="134"/>
+      <c r="C39" s="136"/>
+      <c r="D39" s="136"/>
+      <c r="E39" s="137"/>
       <c r="F39" s="23" t="s">
         <v>28</v>
       </c>
@@ -12178,12 +12186,12 @@
       <c r="GV39" s="13"/>
     </row>
     <row r="40" spans="2:204" ht="26.25">
-      <c r="B40" s="130" t="s">
+      <c r="B40" s="133" t="s">
         <v>89</v>
       </c>
-      <c r="C40" s="131"/>
-      <c r="D40" s="131"/>
-      <c r="E40" s="132"/>
+      <c r="C40" s="134"/>
+      <c r="D40" s="134"/>
+      <c r="E40" s="135"/>
       <c r="F40" s="64"/>
       <c r="G40" s="26"/>
       <c r="H40" s="119" t="s">
@@ -12390,20 +12398,20 @@
       <c r="GU40" s="13"/>
       <c r="GV40" s="13"/>
     </row>
-    <row r="41" spans="2:204" ht="26.25">
-      <c r="B41" s="139"/>
-      <c r="C41" s="130" t="s">
+    <row r="41" spans="2:204" ht="26.25" hidden="1">
+      <c r="B41" s="142"/>
+      <c r="C41" s="133" t="s">
         <v>83</v>
       </c>
-      <c r="D41" s="131"/>
-      <c r="E41" s="132"/>
+      <c r="D41" s="134"/>
+      <c r="E41" s="135"/>
       <c r="F41" s="64"/>
       <c r="G41" s="26"/>
       <c r="H41" s="119" t="s">
         <v>315</v>
       </c>
-      <c r="I41" s="190">
-        <v>44656</v>
+      <c r="I41" s="132" t="s">
+        <v>150</v>
       </c>
       <c r="J41" s="14">
         <v>4</v>
@@ -12605,20 +12613,20 @@
       <c r="GU41" s="13"/>
       <c r="GV41" s="13"/>
     </row>
-    <row r="42" spans="2:204" ht="26.25">
-      <c r="B42" s="140"/>
-      <c r="C42" s="130" t="s">
+    <row r="42" spans="2:204" ht="26.25" hidden="1">
+      <c r="B42" s="143"/>
+      <c r="C42" s="133" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="131"/>
-      <c r="E42" s="132"/>
+      <c r="D42" s="134"/>
+      <c r="E42" s="135"/>
       <c r="F42" s="64"/>
       <c r="G42" s="26"/>
       <c r="H42" s="119" t="s">
         <v>315</v>
       </c>
-      <c r="I42" s="190">
-        <v>44656</v>
+      <c r="I42" s="132" t="s">
+        <v>150</v>
       </c>
       <c r="J42" s="14">
         <v>5</v>
@@ -12821,18 +12829,18 @@
       <c r="GV42" s="13"/>
     </row>
     <row r="43" spans="2:204" ht="26.25">
-      <c r="B43" s="140"/>
-      <c r="C43" s="130" t="s">
+      <c r="B43" s="143"/>
+      <c r="C43" s="133" t="s">
         <v>85</v>
       </c>
-      <c r="D43" s="131"/>
-      <c r="E43" s="132"/>
+      <c r="D43" s="134"/>
+      <c r="E43" s="135"/>
       <c r="F43" s="64"/>
       <c r="G43" s="26"/>
       <c r="H43" s="119" t="s">
         <v>315</v>
       </c>
-      <c r="I43" s="190">
+      <c r="I43" s="131">
         <v>44657</v>
       </c>
       <c r="J43" s="14">
@@ -13036,18 +13044,18 @@
       <c r="GV43" s="13"/>
     </row>
     <row r="44" spans="2:204" ht="30" customHeight="1">
-      <c r="B44" s="140"/>
-      <c r="C44" s="130" t="s">
+      <c r="B44" s="143"/>
+      <c r="C44" s="133" t="s">
         <v>86</v>
       </c>
-      <c r="D44" s="131"/>
-      <c r="E44" s="132"/>
+      <c r="D44" s="134"/>
+      <c r="E44" s="135"/>
       <c r="F44" s="64"/>
       <c r="G44" s="26"/>
       <c r="H44" s="119" t="s">
         <v>315</v>
       </c>
-      <c r="I44" s="190">
+      <c r="I44" s="131">
         <v>44658</v>
       </c>
       <c r="J44" s="14">
@@ -13251,18 +13259,18 @@
       <c r="GV44" s="13"/>
     </row>
     <row r="45" spans="2:204" ht="26.25">
-      <c r="B45" s="140"/>
-      <c r="C45" s="130" t="s">
+      <c r="B45" s="143"/>
+      <c r="C45" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="D45" s="131"/>
-      <c r="E45" s="132"/>
+      <c r="D45" s="134"/>
+      <c r="E45" s="135"/>
       <c r="F45" s="64"/>
       <c r="G45" s="26"/>
       <c r="H45" s="119" t="s">
         <v>315</v>
       </c>
-      <c r="I45" s="190">
+      <c r="I45" s="131">
         <v>44658</v>
       </c>
       <c r="J45" s="14">
@@ -13466,18 +13474,18 @@
       <c r="GV45" s="13"/>
     </row>
     <row r="46" spans="2:204" ht="37.5" customHeight="1">
-      <c r="B46" s="141"/>
-      <c r="C46" s="130" t="s">
+      <c r="B46" s="144"/>
+      <c r="C46" s="133" t="s">
         <v>88</v>
       </c>
-      <c r="D46" s="131"/>
-      <c r="E46" s="132"/>
+      <c r="D46" s="134"/>
+      <c r="E46" s="135"/>
       <c r="F46" s="64"/>
       <c r="G46" s="26"/>
       <c r="H46" s="119" t="s">
         <v>315</v>
       </c>
-      <c r="I46" s="190">
+      <c r="I46" s="131">
         <v>44659</v>
       </c>
       <c r="J46" s="14">
@@ -13681,12 +13689,12 @@
       <c r="GV46" s="13"/>
     </row>
     <row r="47" spans="2:204" ht="26.25">
-      <c r="B47" s="130" t="s">
+      <c r="B47" s="133" t="s">
         <v>90</v>
       </c>
-      <c r="C47" s="131"/>
-      <c r="D47" s="131"/>
-      <c r="E47" s="132"/>
+      <c r="C47" s="134"/>
+      <c r="D47" s="134"/>
+      <c r="E47" s="135"/>
       <c r="F47" s="64"/>
       <c r="G47" s="26"/>
       <c r="H47" s="119" t="s">
@@ -13895,11 +13903,11 @@
     </row>
     <row r="48" spans="2:204" ht="39" customHeight="1">
       <c r="B48" s="65"/>
-      <c r="C48" s="130" t="s">
+      <c r="C48" s="133" t="s">
         <v>92</v>
       </c>
-      <c r="D48" s="131"/>
-      <c r="E48" s="132"/>
+      <c r="D48" s="134"/>
+      <c r="E48" s="135"/>
       <c r="F48" s="64"/>
       <c r="G48" s="26"/>
       <c r="H48" s="119" t="s">
@@ -14107,12 +14115,12 @@
       <c r="GV48" s="13"/>
     </row>
     <row r="49" spans="2:204" ht="26.25">
-      <c r="B49" s="130" t="s">
+      <c r="B49" s="133" t="s">
         <v>91</v>
       </c>
-      <c r="C49" s="131"/>
-      <c r="D49" s="131"/>
-      <c r="E49" s="132"/>
+      <c r="C49" s="134"/>
+      <c r="D49" s="134"/>
+      <c r="E49" s="135"/>
       <c r="F49" s="64"/>
       <c r="G49" s="26"/>
       <c r="H49" s="119" t="s">
@@ -14320,12 +14328,12 @@
       <c r="GV49" s="13"/>
     </row>
     <row r="50" spans="2:204" ht="33.75" customHeight="1">
-      <c r="B50" s="135"/>
-      <c r="C50" s="130" t="s">
+      <c r="B50" s="138"/>
+      <c r="C50" s="133" t="s">
         <v>93</v>
       </c>
-      <c r="D50" s="131"/>
-      <c r="E50" s="132"/>
+      <c r="D50" s="134"/>
+      <c r="E50" s="135"/>
       <c r="F50" s="64"/>
       <c r="G50" s="26"/>
       <c r="H50" s="119" t="s">
@@ -14533,12 +14541,12 @@
       <c r="GV50" s="13"/>
     </row>
     <row r="51" spans="2:204" ht="26.25">
-      <c r="B51" s="138"/>
-      <c r="C51" s="130" t="s">
+      <c r="B51" s="141"/>
+      <c r="C51" s="133" t="s">
         <v>94</v>
       </c>
-      <c r="D51" s="131"/>
-      <c r="E51" s="132"/>
+      <c r="D51" s="134"/>
+      <c r="E51" s="135"/>
       <c r="F51" s="64"/>
       <c r="G51" s="26"/>
       <c r="H51" s="119" t="s">
@@ -14746,12 +14754,12 @@
       <c r="GV51" s="13"/>
     </row>
     <row r="52" spans="2:204" ht="26.25">
-      <c r="B52" s="138"/>
-      <c r="C52" s="130" t="s">
+      <c r="B52" s="141"/>
+      <c r="C52" s="133" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="131"/>
-      <c r="E52" s="132"/>
+      <c r="D52" s="134"/>
+      <c r="E52" s="135"/>
       <c r="F52" s="64"/>
       <c r="G52" s="26"/>
       <c r="H52" s="119" t="s">
@@ -14959,12 +14967,12 @@
       <c r="GV52" s="13"/>
     </row>
     <row r="53" spans="2:204" ht="32.25" customHeight="1">
-      <c r="B53" s="138"/>
-      <c r="C53" s="130" t="s">
+      <c r="B53" s="141"/>
+      <c r="C53" s="133" t="s">
         <v>98</v>
       </c>
-      <c r="D53" s="131"/>
-      <c r="E53" s="132"/>
+      <c r="D53" s="134"/>
+      <c r="E53" s="135"/>
       <c r="F53" s="64"/>
       <c r="G53" s="26"/>
       <c r="H53" s="119" t="s">
@@ -15172,12 +15180,12 @@
       <c r="GV53" s="13"/>
     </row>
     <row r="54" spans="2:204" ht="43.5" customHeight="1">
-      <c r="B54" s="138"/>
-      <c r="C54" s="130" t="s">
+      <c r="B54" s="141"/>
+      <c r="C54" s="133" t="s">
         <v>95</v>
       </c>
-      <c r="D54" s="131"/>
-      <c r="E54" s="132"/>
+      <c r="D54" s="134"/>
+      <c r="E54" s="135"/>
       <c r="F54" s="64"/>
       <c r="G54" s="26"/>
       <c r="H54" s="119" t="s">
@@ -15385,12 +15393,12 @@
       <c r="GV54" s="13"/>
     </row>
     <row r="55" spans="2:204" ht="43.5" customHeight="1">
-      <c r="B55" s="138"/>
-      <c r="C55" s="130" t="s">
+      <c r="B55" s="141"/>
+      <c r="C55" s="133" t="s">
         <v>96</v>
       </c>
-      <c r="D55" s="131"/>
-      <c r="E55" s="132"/>
+      <c r="D55" s="134"/>
+      <c r="E55" s="135"/>
       <c r="F55" s="64"/>
       <c r="G55" s="26"/>
       <c r="H55" s="119" t="s">
@@ -15598,12 +15606,12 @@
       <c r="GV55" s="13"/>
     </row>
     <row r="56" spans="2:204" ht="33.75" customHeight="1">
-      <c r="B56" s="138"/>
-      <c r="C56" s="130" t="s">
+      <c r="B56" s="141"/>
+      <c r="C56" s="133" t="s">
         <v>97</v>
       </c>
-      <c r="D56" s="131"/>
-      <c r="E56" s="132"/>
+      <c r="D56" s="134"/>
+      <c r="E56" s="135"/>
       <c r="F56" s="64"/>
       <c r="G56" s="26"/>
       <c r="H56" s="119" t="s">
@@ -15811,12 +15819,12 @@
       <c r="GV56" s="13"/>
     </row>
     <row r="57" spans="2:204" ht="26.25">
-      <c r="B57" s="138"/>
-      <c r="C57" s="130" t="s">
+      <c r="B57" s="141"/>
+      <c r="C57" s="133" t="s">
         <v>113</v>
       </c>
-      <c r="D57" s="131"/>
-      <c r="E57" s="132"/>
+      <c r="D57" s="134"/>
+      <c r="E57" s="135"/>
       <c r="F57" s="64"/>
       <c r="G57" s="26"/>
       <c r="H57" s="119" t="s">
@@ -16024,12 +16032,12 @@
       <c r="GV57" s="13"/>
     </row>
     <row r="58" spans="2:204" ht="26.25">
-      <c r="B58" s="138"/>
-      <c r="C58" s="135"/>
-      <c r="D58" s="142" t="s">
+      <c r="B58" s="141"/>
+      <c r="C58" s="138"/>
+      <c r="D58" s="145" t="s">
         <v>100</v>
       </c>
-      <c r="E58" s="143"/>
+      <c r="E58" s="146"/>
       <c r="F58" s="64"/>
       <c r="G58" s="26"/>
       <c r="H58" s="119" t="s">
@@ -16237,12 +16245,12 @@
       <c r="GV58" s="13"/>
     </row>
     <row r="59" spans="2:204" ht="26.25">
-      <c r="B59" s="138"/>
-      <c r="C59" s="138"/>
-      <c r="D59" s="142" t="s">
+      <c r="B59" s="141"/>
+      <c r="C59" s="141"/>
+      <c r="D59" s="145" t="s">
         <v>102</v>
       </c>
-      <c r="E59" s="143"/>
+      <c r="E59" s="146"/>
       <c r="F59" s="64"/>
       <c r="G59" s="26"/>
       <c r="H59" s="119" t="s">
@@ -16450,9 +16458,9 @@
       <c r="GV59" s="13"/>
     </row>
     <row r="60" spans="2:204" ht="36" customHeight="1">
-      <c r="B60" s="138"/>
-      <c r="C60" s="138"/>
-      <c r="D60" s="135"/>
+      <c r="B60" s="141"/>
+      <c r="C60" s="141"/>
+      <c r="D60" s="138"/>
       <c r="E60" s="65" t="s">
         <v>105</v>
       </c>
@@ -16663,9 +16671,9 @@
       <c r="GV60" s="13"/>
     </row>
     <row r="61" spans="2:204" ht="35.25" customHeight="1">
-      <c r="B61" s="138"/>
-      <c r="C61" s="138"/>
-      <c r="D61" s="138"/>
+      <c r="B61" s="141"/>
+      <c r="C61" s="141"/>
+      <c r="D61" s="141"/>
       <c r="E61" s="65" t="s">
         <v>106</v>
       </c>
@@ -16876,9 +16884,9 @@
       <c r="GV61" s="13"/>
     </row>
     <row r="62" spans="2:204" ht="35.25" customHeight="1">
-      <c r="B62" s="138"/>
-      <c r="C62" s="138"/>
-      <c r="D62" s="138"/>
+      <c r="B62" s="141"/>
+      <c r="C62" s="141"/>
+      <c r="D62" s="141"/>
       <c r="E62" s="65" t="s">
         <v>108</v>
       </c>
@@ -17089,9 +17097,9 @@
       <c r="GV62" s="13"/>
     </row>
     <row r="63" spans="2:204" ht="33.75" customHeight="1">
-      <c r="B63" s="138"/>
-      <c r="C63" s="138"/>
-      <c r="D63" s="138"/>
+      <c r="B63" s="141"/>
+      <c r="C63" s="141"/>
+      <c r="D63" s="141"/>
       <c r="E63" s="65" t="s">
         <v>112</v>
       </c>
@@ -17302,9 +17310,9 @@
       <c r="GV63" s="13"/>
     </row>
     <row r="64" spans="2:204" ht="26.25">
-      <c r="B64" s="138"/>
-      <c r="C64" s="138"/>
-      <c r="D64" s="138"/>
+      <c r="B64" s="141"/>
+      <c r="C64" s="141"/>
+      <c r="D64" s="141"/>
       <c r="E64" s="65" t="s">
         <v>107</v>
       </c>
@@ -17515,9 +17523,9 @@
       <c r="GV64" s="13"/>
     </row>
     <row r="65" spans="1:204" ht="26.25">
-      <c r="B65" s="138"/>
-      <c r="C65" s="138"/>
-      <c r="D65" s="138"/>
+      <c r="B65" s="141"/>
+      <c r="C65" s="141"/>
+      <c r="D65" s="141"/>
       <c r="E65" s="65" t="s">
         <v>109</v>
       </c>
@@ -17728,9 +17736,9 @@
       <c r="GV65" s="13"/>
     </row>
     <row r="66" spans="1:204" ht="26.25">
-      <c r="B66" s="138"/>
-      <c r="C66" s="138"/>
-      <c r="D66" s="138"/>
+      <c r="B66" s="141"/>
+      <c r="C66" s="141"/>
+      <c r="D66" s="141"/>
       <c r="E66" s="65" t="s">
         <v>110</v>
       </c>
@@ -17941,9 +17949,9 @@
       <c r="GV66" s="13"/>
     </row>
     <row r="67" spans="1:204" ht="37.5" customHeight="1">
-      <c r="B67" s="138"/>
-      <c r="C67" s="138"/>
-      <c r="D67" s="136"/>
+      <c r="B67" s="141"/>
+      <c r="C67" s="141"/>
+      <c r="D67" s="139"/>
       <c r="E67" s="65" t="s">
         <v>111</v>
       </c>
@@ -18154,12 +18162,12 @@
       <c r="GV67" s="13"/>
     </row>
     <row r="68" spans="1:204" ht="33" customHeight="1">
-      <c r="B68" s="138"/>
-      <c r="C68" s="138"/>
-      <c r="D68" s="130" t="s">
+      <c r="B68" s="141"/>
+      <c r="C68" s="141"/>
+      <c r="D68" s="133" t="s">
         <v>101</v>
       </c>
-      <c r="E68" s="132"/>
+      <c r="E68" s="135"/>
       <c r="F68" s="64"/>
       <c r="G68" s="26"/>
       <c r="H68" s="119" t="s">
@@ -18367,12 +18375,12 @@
       <c r="GV68" s="13"/>
     </row>
     <row r="69" spans="1:204" ht="26.25">
-      <c r="B69" s="138"/>
-      <c r="C69" s="138"/>
-      <c r="D69" s="130" t="s">
+      <c r="B69" s="141"/>
+      <c r="C69" s="141"/>
+      <c r="D69" s="133" t="s">
         <v>103</v>
       </c>
-      <c r="E69" s="132"/>
+      <c r="E69" s="135"/>
       <c r="F69" s="64"/>
       <c r="G69" s="26"/>
       <c r="H69" s="119" t="s">
@@ -18580,12 +18588,12 @@
       <c r="GV69" s="13"/>
     </row>
     <row r="70" spans="1:204" ht="34.5" customHeight="1">
-      <c r="B70" s="136"/>
-      <c r="C70" s="136"/>
-      <c r="D70" s="130" t="s">
+      <c r="B70" s="139"/>
+      <c r="C70" s="139"/>
+      <c r="D70" s="133" t="s">
         <v>104</v>
       </c>
-      <c r="E70" s="132"/>
+      <c r="E70" s="135"/>
       <c r="F70" s="64"/>
       <c r="G70" s="26"/>
       <c r="H70" s="119" t="s">
@@ -18793,12 +18801,12 @@
       <c r="GV70" s="13"/>
     </row>
     <row r="71" spans="1:204" ht="26.25">
-      <c r="B71" s="144" t="s">
+      <c r="B71" s="147" t="s">
         <v>51</v>
       </c>
-      <c r="C71" s="133"/>
-      <c r="D71" s="133"/>
-      <c r="E71" s="134"/>
+      <c r="C71" s="136"/>
+      <c r="D71" s="136"/>
+      <c r="E71" s="137"/>
       <c r="F71" s="23" t="s">
         <v>27</v>
       </c>
@@ -19016,10 +19024,10 @@
     <row r="72" spans="1:204" ht="45" customHeight="1">
       <c r="B72" s="97"/>
       <c r="C72" s="98"/>
-      <c r="D72" s="137" t="s">
+      <c r="D72" s="140" t="s">
         <v>312</v>
       </c>
-      <c r="E72" s="137"/>
+      <c r="E72" s="140"/>
       <c r="F72" s="114"/>
       <c r="G72" s="26"/>
       <c r="H72" s="119" t="s">
@@ -19229,10 +19237,10 @@
     <row r="73" spans="1:204" ht="47.25" customHeight="1">
       <c r="B73" s="97"/>
       <c r="C73" s="98"/>
-      <c r="D73" s="137" t="s">
+      <c r="D73" s="140" t="s">
         <v>313</v>
       </c>
-      <c r="E73" s="137"/>
+      <c r="E73" s="140"/>
       <c r="F73" s="64"/>
       <c r="G73" s="26"/>
       <c r="H73" s="119" t="s">
@@ -19442,10 +19450,10 @@
     <row r="74" spans="1:204" ht="26.25">
       <c r="B74" s="97"/>
       <c r="C74" s="98"/>
-      <c r="D74" s="137" t="s">
+      <c r="D74" s="140" t="s">
         <v>314</v>
       </c>
-      <c r="E74" s="137"/>
+      <c r="E74" s="140"/>
       <c r="F74" s="64"/>
       <c r="G74" s="26"/>
       <c r="H74" s="119" t="s">
@@ -19656,12 +19664,12 @@
       <c r="A75" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B75" s="145" t="s">
+      <c r="B75" s="148" t="s">
         <v>320</v>
       </c>
-      <c r="C75" s="146"/>
-      <c r="D75" s="146"/>
-      <c r="E75" s="146"/>
+      <c r="C75" s="149"/>
+      <c r="D75" s="149"/>
+      <c r="E75" s="149"/>
       <c r="F75" s="27"/>
       <c r="G75" s="7"/>
       <c r="H75" s="8"/>
@@ -19863,12 +19871,12 @@
       <c r="GV75" s="13"/>
     </row>
     <row r="76" spans="1:204" ht="26.25">
-      <c r="B76" s="144" t="s">
+      <c r="B76" s="147" t="s">
         <v>49</v>
       </c>
-      <c r="C76" s="133"/>
-      <c r="D76" s="133"/>
-      <c r="E76" s="134"/>
+      <c r="C76" s="136"/>
+      <c r="D76" s="136"/>
+      <c r="E76" s="137"/>
       <c r="F76" s="23" t="s">
         <v>31</v>
       </c>
@@ -20085,11 +20093,11 @@
     </row>
     <row r="77" spans="1:204" ht="44.25" customHeight="1">
       <c r="B77" s="97"/>
-      <c r="C77" s="133" t="s">
+      <c r="C77" s="136" t="s">
         <v>298</v>
       </c>
-      <c r="D77" s="133"/>
-      <c r="E77" s="134"/>
+      <c r="D77" s="136"/>
+      <c r="E77" s="137"/>
       <c r="F77" s="23"/>
       <c r="G77" s="26"/>
       <c r="H77" s="14" t="s">
@@ -20298,11 +20306,11 @@
     </row>
     <row r="78" spans="1:204" ht="60.75" customHeight="1">
       <c r="B78" s="97"/>
-      <c r="C78" s="133" t="s">
+      <c r="C78" s="136" t="s">
         <v>304</v>
       </c>
-      <c r="D78" s="133"/>
-      <c r="E78" s="134"/>
+      <c r="D78" s="136"/>
+      <c r="E78" s="137"/>
       <c r="F78" s="23"/>
       <c r="G78" s="26"/>
       <c r="H78" s="14" t="s">
@@ -20511,11 +20519,11 @@
     </row>
     <row r="79" spans="1:204" ht="26.25">
       <c r="B79" s="97"/>
-      <c r="C79" s="133" t="s">
+      <c r="C79" s="136" t="s">
         <v>283</v>
       </c>
-      <c r="D79" s="133"/>
-      <c r="E79" s="134"/>
+      <c r="D79" s="136"/>
+      <c r="E79" s="137"/>
       <c r="F79" s="23"/>
       <c r="G79" s="26"/>
       <c r="H79" s="14" t="s">
@@ -20724,11 +20732,11 @@
     </row>
     <row r="80" spans="1:204" ht="26.25">
       <c r="B80" s="97"/>
-      <c r="C80" s="133" t="s">
+      <c r="C80" s="136" t="s">
         <v>284</v>
       </c>
-      <c r="D80" s="133"/>
-      <c r="E80" s="134"/>
+      <c r="D80" s="136"/>
+      <c r="E80" s="137"/>
       <c r="F80" s="23"/>
       <c r="G80" s="26"/>
       <c r="H80" s="14" t="s">
@@ -20936,12 +20944,12 @@
       <c r="GV80" s="13"/>
     </row>
     <row r="81" spans="1:204" ht="26.25">
-      <c r="B81" s="144" t="s">
+      <c r="B81" s="147" t="s">
         <v>50</v>
       </c>
-      <c r="C81" s="133"/>
-      <c r="D81" s="133"/>
-      <c r="E81" s="134"/>
+      <c r="C81" s="136"/>
+      <c r="D81" s="136"/>
+      <c r="E81" s="137"/>
       <c r="F81" s="23" t="s">
         <v>28</v>
       </c>
@@ -21158,11 +21166,11 @@
     </row>
     <row r="82" spans="1:204" ht="48.75" customHeight="1">
       <c r="B82" s="97"/>
-      <c r="C82" s="133" t="s">
+      <c r="C82" s="136" t="s">
         <v>285</v>
       </c>
-      <c r="D82" s="133"/>
-      <c r="E82" s="134"/>
+      <c r="D82" s="136"/>
+      <c r="E82" s="137"/>
       <c r="F82" s="23"/>
       <c r="G82" s="26"/>
       <c r="H82" s="119" t="s">
@@ -21371,11 +21379,11 @@
     </row>
     <row r="83" spans="1:204" ht="26.25">
       <c r="B83" s="97"/>
-      <c r="C83" s="133" t="s">
+      <c r="C83" s="136" t="s">
         <v>286</v>
       </c>
-      <c r="D83" s="133"/>
-      <c r="E83" s="134"/>
+      <c r="D83" s="136"/>
+      <c r="E83" s="137"/>
       <c r="F83" s="23"/>
       <c r="G83" s="26"/>
       <c r="H83" s="119" t="s">
@@ -21583,12 +21591,12 @@
       <c r="GV83" s="13"/>
     </row>
     <row r="84" spans="1:204" ht="26.25">
-      <c r="B84" s="144" t="s">
+      <c r="B84" s="147" t="s">
         <v>280</v>
       </c>
-      <c r="C84" s="133"/>
-      <c r="D84" s="133"/>
-      <c r="E84" s="134"/>
+      <c r="C84" s="136"/>
+      <c r="D84" s="136"/>
+      <c r="E84" s="137"/>
       <c r="F84" s="47" t="s">
         <v>39</v>
       </c>
@@ -21804,12 +21812,12 @@
       <c r="GV84" s="13"/>
     </row>
     <row r="85" spans="1:204" ht="26.25">
-      <c r="B85" s="144" t="s">
+      <c r="B85" s="147" t="s">
         <v>281</v>
       </c>
-      <c r="C85" s="133"/>
-      <c r="D85" s="133"/>
-      <c r="E85" s="134"/>
+      <c r="C85" s="136"/>
+      <c r="D85" s="136"/>
+      <c r="E85" s="137"/>
       <c r="F85" s="23" t="s">
         <v>42</v>
       </c>
@@ -22025,12 +22033,12 @@
       <c r="GV85" s="13"/>
     </row>
     <row r="86" spans="1:204" ht="26.25">
-      <c r="B86" s="157"/>
-      <c r="C86" s="158"/>
-      <c r="D86" s="155" t="s">
+      <c r="B86" s="160"/>
+      <c r="C86" s="161"/>
+      <c r="D86" s="158" t="s">
         <v>291</v>
       </c>
-      <c r="E86" s="134"/>
+      <c r="E86" s="137"/>
       <c r="F86" s="23"/>
       <c r="G86" s="26"/>
       <c r="H86" s="122" t="s">
@@ -22238,8 +22246,8 @@
       <c r="GV86" s="13"/>
     </row>
     <row r="87" spans="1:204" ht="30" customHeight="1">
-      <c r="B87" s="159"/>
-      <c r="C87" s="160"/>
+      <c r="B87" s="162"/>
+      <c r="C87" s="163"/>
       <c r="D87" s="123"/>
       <c r="E87" s="99" t="s">
         <v>292</v>
@@ -22451,12 +22459,12 @@
       <c r="GV87" s="13"/>
     </row>
     <row r="88" spans="1:204" ht="26.25">
-      <c r="B88" s="159"/>
-      <c r="C88" s="161"/>
-      <c r="D88" s="156" t="s">
+      <c r="B88" s="162"/>
+      <c r="C88" s="164"/>
+      <c r="D88" s="159" t="s">
         <v>290</v>
       </c>
-      <c r="E88" s="134"/>
+      <c r="E88" s="137"/>
       <c r="F88" s="23"/>
       <c r="G88" s="26"/>
       <c r="H88" s="14"/>
@@ -22662,9 +22670,9 @@
       <c r="GV88" s="13"/>
     </row>
     <row r="89" spans="1:204" ht="49.5" customHeight="1">
-      <c r="B89" s="159"/>
-      <c r="C89" s="160"/>
-      <c r="D89" s="164"/>
+      <c r="B89" s="162"/>
+      <c r="C89" s="163"/>
+      <c r="D89" s="167"/>
       <c r="E89" s="99" t="s">
         <v>288</v>
       </c>
@@ -22875,9 +22883,9 @@
       <c r="GV89" s="13"/>
     </row>
     <row r="90" spans="1:204" ht="28.5" customHeight="1">
-      <c r="B90" s="162"/>
-      <c r="C90" s="163"/>
-      <c r="D90" s="165"/>
+      <c r="B90" s="165"/>
+      <c r="C90" s="166"/>
+      <c r="D90" s="168"/>
       <c r="E90" s="99" t="s">
         <v>289</v>
       </c>
@@ -23088,12 +23096,12 @@
       <c r="GV90" s="13"/>
     </row>
     <row r="91" spans="1:204" ht="26.25">
-      <c r="B91" s="144" t="s">
+      <c r="B91" s="147" t="s">
         <v>282</v>
       </c>
-      <c r="C91" s="133"/>
-      <c r="D91" s="152"/>
-      <c r="E91" s="134"/>
+      <c r="C91" s="136"/>
+      <c r="D91" s="155"/>
+      <c r="E91" s="137"/>
       <c r="F91" s="23" t="s">
         <v>29</v>
       </c>
@@ -23311,10 +23319,10 @@
     <row r="92" spans="1:204" ht="47.25" customHeight="1">
       <c r="B92" s="97"/>
       <c r="C92" s="98"/>
-      <c r="D92" s="133" t="s">
+      <c r="D92" s="136" t="s">
         <v>316</v>
       </c>
-      <c r="E92" s="134"/>
+      <c r="E92" s="137"/>
       <c r="F92" s="114"/>
       <c r="G92" s="46"/>
       <c r="H92" s="115" t="s">
@@ -23524,10 +23532,10 @@
     <row r="93" spans="1:204" ht="27" customHeight="1">
       <c r="B93" s="97"/>
       <c r="C93" s="98"/>
-      <c r="D93" s="133" t="s">
+      <c r="D93" s="136" t="s">
         <v>317</v>
       </c>
-      <c r="E93" s="134"/>
+      <c r="E93" s="137"/>
       <c r="F93" s="114"/>
       <c r="G93" s="46"/>
       <c r="H93" s="115" t="s">
@@ -23738,12 +23746,12 @@
       <c r="A94" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B94" s="153" t="s">
+      <c r="B94" s="156" t="s">
         <v>319</v>
       </c>
-      <c r="C94" s="154"/>
-      <c r="D94" s="154"/>
-      <c r="E94" s="154"/>
+      <c r="C94" s="157"/>
+      <c r="D94" s="157"/>
+      <c r="E94" s="157"/>
       <c r="F94" s="27"/>
       <c r="G94" s="7"/>
       <c r="H94" s="8"/>
@@ -23949,12 +23957,12 @@
       <c r="GV94" s="13"/>
     </row>
     <row r="95" spans="1:204" ht="26.25">
-      <c r="B95" s="144" t="s">
+      <c r="B95" s="147" t="s">
         <v>49</v>
       </c>
-      <c r="C95" s="133"/>
-      <c r="D95" s="133"/>
-      <c r="E95" s="134"/>
+      <c r="C95" s="136"/>
+      <c r="D95" s="136"/>
+      <c r="E95" s="137"/>
       <c r="F95" s="23" t="s">
         <v>31</v>
       </c>
@@ -24171,11 +24179,11 @@
     </row>
     <row r="96" spans="1:204" ht="48" customHeight="1">
       <c r="B96" s="97"/>
-      <c r="C96" s="133" t="s">
+      <c r="C96" s="136" t="s">
         <v>303</v>
       </c>
-      <c r="D96" s="133"/>
-      <c r="E96" s="134"/>
+      <c r="D96" s="136"/>
+      <c r="E96" s="137"/>
       <c r="F96" s="23"/>
       <c r="G96" s="16"/>
       <c r="H96" s="119" t="s">
@@ -24384,11 +24392,11 @@
     </row>
     <row r="97" spans="2:204" ht="26.25">
       <c r="B97" s="97"/>
-      <c r="C97" s="133" t="s">
+      <c r="C97" s="136" t="s">
         <v>305</v>
       </c>
-      <c r="D97" s="133"/>
-      <c r="E97" s="134"/>
+      <c r="D97" s="136"/>
+      <c r="E97" s="137"/>
       <c r="F97" s="23"/>
       <c r="G97" s="16"/>
       <c r="H97" s="119" t="s">
@@ -24597,11 +24605,11 @@
     </row>
     <row r="98" spans="2:204" ht="26.25">
       <c r="B98" s="97"/>
-      <c r="C98" s="133" t="s">
+      <c r="C98" s="136" t="s">
         <v>306</v>
       </c>
-      <c r="D98" s="133"/>
-      <c r="E98" s="134"/>
+      <c r="D98" s="136"/>
+      <c r="E98" s="137"/>
       <c r="F98" s="23"/>
       <c r="G98" s="16"/>
       <c r="H98" s="119" t="s">
@@ -24810,11 +24818,11 @@
     </row>
     <row r="99" spans="2:204" ht="26.25">
       <c r="B99" s="97"/>
-      <c r="C99" s="133" t="s">
+      <c r="C99" s="136" t="s">
         <v>283</v>
       </c>
-      <c r="D99" s="133"/>
-      <c r="E99" s="134"/>
+      <c r="D99" s="136"/>
+      <c r="E99" s="137"/>
       <c r="F99" s="23"/>
       <c r="G99" s="16"/>
       <c r="H99" s="119" t="s">
@@ -25023,11 +25031,11 @@
     </row>
     <row r="100" spans="2:204" ht="26.25">
       <c r="B100" s="97"/>
-      <c r="C100" s="133" t="s">
+      <c r="C100" s="136" t="s">
         <v>318</v>
       </c>
-      <c r="D100" s="133"/>
-      <c r="E100" s="134"/>
+      <c r="D100" s="136"/>
+      <c r="E100" s="137"/>
       <c r="F100" s="23"/>
       <c r="G100" s="26"/>
       <c r="H100" s="14" t="s">
@@ -25235,12 +25243,12 @@
       <c r="GV100" s="13"/>
     </row>
     <row r="101" spans="2:204" ht="26.25">
-      <c r="B101" s="144" t="s">
+      <c r="B101" s="147" t="s">
         <v>50</v>
       </c>
-      <c r="C101" s="133"/>
-      <c r="D101" s="133"/>
-      <c r="E101" s="134"/>
+      <c r="C101" s="136"/>
+      <c r="D101" s="136"/>
+      <c r="E101" s="137"/>
       <c r="F101" s="23" t="s">
         <v>28</v>
       </c>
@@ -25455,11 +25463,11 @@
     </row>
     <row r="102" spans="2:204" ht="48.75" customHeight="1">
       <c r="B102" s="97"/>
-      <c r="C102" s="133" t="s">
+      <c r="C102" s="136" t="s">
         <v>285</v>
       </c>
-      <c r="D102" s="133"/>
-      <c r="E102" s="134"/>
+      <c r="D102" s="136"/>
+      <c r="E102" s="137"/>
       <c r="F102" s="23"/>
       <c r="G102" s="26"/>
       <c r="H102" s="119" t="s">
@@ -25668,11 +25676,11 @@
     </row>
     <row r="103" spans="2:204" ht="26.25">
       <c r="B103" s="97"/>
-      <c r="C103" s="133" t="s">
+      <c r="C103" s="136" t="s">
         <v>311</v>
       </c>
-      <c r="D103" s="133"/>
-      <c r="E103" s="134"/>
+      <c r="D103" s="136"/>
+      <c r="E103" s="137"/>
       <c r="F103" s="23"/>
       <c r="G103" s="26"/>
       <c r="H103" s="119" t="s">
@@ -25880,12 +25888,12 @@
       <c r="GV103" s="13"/>
     </row>
     <row r="104" spans="2:204" ht="26.25">
-      <c r="B104" s="144" t="s">
+      <c r="B104" s="147" t="s">
         <v>299</v>
       </c>
-      <c r="C104" s="133"/>
-      <c r="D104" s="133"/>
-      <c r="E104" s="134"/>
+      <c r="C104" s="136"/>
+      <c r="D104" s="136"/>
+      <c r="E104" s="137"/>
       <c r="F104" s="47" t="s">
         <v>39</v>
       </c>
@@ -26099,12 +26107,12 @@
       <c r="GV104" s="13"/>
     </row>
     <row r="105" spans="2:204" ht="32.25">
-      <c r="B105" s="144" t="s">
+      <c r="B105" s="147" t="s">
         <v>300</v>
       </c>
-      <c r="C105" s="133"/>
-      <c r="D105" s="133"/>
-      <c r="E105" s="134"/>
+      <c r="C105" s="136"/>
+      <c r="D105" s="136"/>
+      <c r="E105" s="137"/>
       <c r="F105" s="23" t="s">
         <v>29</v>
       </c>
@@ -26321,11 +26329,11 @@
     </row>
     <row r="106" spans="2:204" ht="26.25">
       <c r="B106" s="97"/>
-      <c r="C106" s="133" t="s">
+      <c r="C106" s="136" t="s">
         <v>307</v>
       </c>
-      <c r="D106" s="133"/>
-      <c r="E106" s="134"/>
+      <c r="D106" s="136"/>
+      <c r="E106" s="137"/>
       <c r="F106" s="23"/>
       <c r="G106" s="46"/>
       <c r="H106" s="14" t="s">
@@ -26534,11 +26542,11 @@
     </row>
     <row r="107" spans="2:204" ht="26.25">
       <c r="B107" s="97"/>
-      <c r="C107" s="133" t="s">
+      <c r="C107" s="136" t="s">
         <v>308</v>
       </c>
-      <c r="D107" s="133"/>
-      <c r="E107" s="134"/>
+      <c r="D107" s="136"/>
+      <c r="E107" s="137"/>
       <c r="F107" s="23"/>
       <c r="G107" s="46"/>
       <c r="H107" s="14" t="s">
@@ -26747,11 +26755,11 @@
     </row>
     <row r="108" spans="2:204" ht="26.25">
       <c r="B108" s="97"/>
-      <c r="C108" s="133" t="s">
+      <c r="C108" s="136" t="s">
         <v>309</v>
       </c>
-      <c r="D108" s="133"/>
-      <c r="E108" s="134"/>
+      <c r="D108" s="136"/>
+      <c r="E108" s="137"/>
       <c r="F108" s="23"/>
       <c r="G108" s="46"/>
       <c r="H108" s="14" t="s">
@@ -26960,11 +26968,11 @@
     </row>
     <row r="109" spans="2:204" ht="26.25">
       <c r="B109" s="97"/>
-      <c r="C109" s="133" t="s">
+      <c r="C109" s="136" t="s">
         <v>310</v>
       </c>
-      <c r="D109" s="133"/>
-      <c r="E109" s="134"/>
+      <c r="D109" s="136"/>
+      <c r="E109" s="137"/>
       <c r="F109" s="23"/>
       <c r="G109" s="46"/>
       <c r="H109" s="14" t="s">
@@ -27172,12 +27180,12 @@
       <c r="GV109" s="13"/>
     </row>
     <row r="110" spans="2:204" ht="26.25">
-      <c r="B110" s="147" t="s">
+      <c r="B110" s="150" t="s">
         <v>301</v>
       </c>
-      <c r="C110" s="146"/>
-      <c r="D110" s="146"/>
-      <c r="E110" s="148"/>
+      <c r="C110" s="149"/>
+      <c r="D110" s="149"/>
+      <c r="E110" s="151"/>
       <c r="F110" s="24"/>
       <c r="G110" s="17"/>
       <c r="H110" s="18" t="s">
@@ -27389,12 +27397,12 @@
       <c r="GV110" s="13"/>
     </row>
     <row r="111" spans="2:204" ht="32.25">
-      <c r="B111" s="147" t="s">
+      <c r="B111" s="150" t="s">
         <v>302</v>
       </c>
-      <c r="C111" s="146"/>
-      <c r="D111" s="146"/>
-      <c r="E111" s="148"/>
+      <c r="C111" s="149"/>
+      <c r="D111" s="149"/>
+      <c r="E111" s="151"/>
       <c r="F111" s="24"/>
       <c r="G111" s="17"/>
       <c r="H111" s="18" t="s">
@@ -27606,10 +27614,10 @@
       <c r="GV111" s="13"/>
     </row>
     <row r="112" spans="2:204" ht="30" customHeight="1">
-      <c r="B112" s="149"/>
-      <c r="C112" s="150"/>
-      <c r="D112" s="150"/>
-      <c r="E112" s="151"/>
+      <c r="B112" s="152"/>
+      <c r="C112" s="153"/>
+      <c r="D112" s="153"/>
+      <c r="E112" s="154"/>
       <c r="F112" s="25"/>
       <c r="G112" s="12"/>
       <c r="H112" s="12"/>

</xml_diff>